<commit_message>
updated mom till date
</commit_message>
<xml_diff>
--- a/Minutes_of_meeting/Minutes-of-meetings.xlsx
+++ b/Minutes_of_meeting/Minutes-of-meetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIRISH\Desktop\US-Stock-Options-Data-Pipeline-microservice\Minutes_of_meeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781609CB-4DFA-433F-8029-F3123A7506CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E3325F-9E25-41FD-8C6C-29269607BE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6626D02-EAB1-4E07-BCA0-63E94328CB3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>DATE</t>
   </si>
@@ -953,6 +953,55 @@
 3. Discussed and implemented necessary edits to merge and smoothen the full demo recording, ensuring consistency in flow and transitions.
 4. Worked collectively on finalizing the presentation script, refining each member’s speaking part for clarity and time management.
 5. Ensured alignment between script, slides, and demo for a cohesive presentation delivery.</t>
+  </si>
+  <si>
+    <t>1. Frontend database integration through Angular was causing technical conflicts and instability.
+2. Lack of abstraction between backend logic and frontend components led to coupling and error propagation.
+3. Some backend services still pending implementation or testing, affecting full-stack flow.</t>
+  </si>
+  <si>
+    <t>1. Reviewed the status of remaining backend services that are yet to be completed.
+2. Discussed data integration efforts for the frontend, including real-time and historical data display.
+3. Identified integration issues between Angular and direct database access, which were causing conflicts.
+4. Agreed that the backend team will create API services to resolve the frontend-backend integration challenge and fetch data.
+5. Planned the next sprint, with tasks assigned based on pending modules and integration goals.</t>
+  </si>
+  <si>
+    <t>1. Backend team to design and deploy API services to expose necessary data for the frontend securely and efficiently.
+2. Frontend team to integrate APIs via Angular services, replacing direct database calls.
+3. Define and assign clear tasks for the next sprint, focusing on:
+a. Completing the remaining backend services,
+b. Finalizing frontend data visualizations,
+c. Ensuring stable integration across modules.
+4. Schedule a follow-up review session to validate progress and prepare for the next project milestone.</t>
+  </si>
+  <si>
+    <t>Reviewed overall progress across frontend, backend, and supporting services.
+1. Backend Update:
+a. Implemented multithreading to efficiently handle 120 stock symbols using 5 Twelve Data API keys, with each key handling 24 symbols every 3 minutes.
+b. Completed the File Writer service.
+c. Data Collector service is successfully pushing B13 to Prometheus and Grafana for monitoring.
+2. Frontend Update:
+a. Successfully integrated APIs to fetch real-time data from backend.
+b. Discussed UI enhancements and remaining adjustments needed on the dashboard layout and presentation.
+3. Identified remaining backend components such as:
+a. B13Load Balancer service
+b. Additional Monitoring and Observability features not yet implemented</t>
+  </si>
+  <si>
+    <t>1. Need to manage API key limits and scheduling efficiently to avoid rate limiting while scaling.
+2. UI adjustments and data mapping on the dashboard required refinement after API integration.
+3. Monitoring setup is partial; Grafana and Prometheus integration is only complete for the data collector, not for other services.</t>
+  </si>
+  <si>
+    <t>1. Backend team to:
+a. Complete Load Balancer implementation.
+b. Extend Prometheus and Grafana integration to remaining services for full-stack observability.
+2. Frontend team to:
+a. Finalize UI changes based on the feedback discussed.
+b. Ensure proper rendering of dynamic data on the dashboard with error handling.
+3. Perform testing for multithreaded data collection, ensuring stability under production load.
+4. Plan next meeting to review full system integration before final delivery milestones</t>
   </si>
 </sst>
 </file>
@@ -1008,17 +1057,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1028,10 +1068,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,37 +1403,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4CB3A1-9D53-459A-9590-285823EBD908}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="17.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:4" ht="405" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="405" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1390,9 +1446,10 @@
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1401,12 +1458,13 @@
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
+      <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>45814</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1418,9 +1476,10 @@
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="285" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>45816</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1432,20 +1491,24 @@
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>45817</v>
       </c>
+      <c r="B6" s="9"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>45820</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1454,12 +1517,13 @@
       <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:5" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>45821</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1468,12 +1532,13 @@
       <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>45824</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1482,12 +1547,13 @@
       <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="360" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:5" ht="360" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>45708</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1496,12 +1562,13 @@
       <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:4" ht="315" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>45831</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1510,12 +1577,36 @@
       <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12"/>
+    <row r="12" spans="1:5" ht="360" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>45835</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13"/>
+    <row r="13" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>45845</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>